<commit_message>
Parallel processing for Monte Carlo
</commit_message>
<xml_diff>
--- a/docs/Examples/EOS_calculations/Fluid_Inclusion_Densities_Example1.xlsx
+++ b/docs/Examples/EOS_calculations/Fluid_Inclusion_Densities_Example1.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\DiadFit_outer\docs\Examples\Example5_FI_density_to_depth\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\Box\Berkeley_new\DiadFit_outer\docs\Examples\EOS_calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1F6CCE-5567-43BF-B901-0FFF05F12E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475E1E85-6E84-4A47-BE64-65311B263320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="1" xr2:uid="{70B86B56-DC75-4A25-AC0B-5B934F645505}"/>
+    <workbookView xWindow="-3630" yWindow="90" windowWidth="20740" windowHeight="13400" activeTab="1" xr2:uid="{70B86B56-DC75-4A25-AC0B-5B934F645505}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Diff_Temps" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
   <si>
     <t>Sample</t>
   </si>
@@ -169,6 +169,66 @@
   </si>
   <si>
     <t>Host_Fo_content</t>
+  </si>
+  <si>
+    <t>FI74</t>
+  </si>
+  <si>
+    <t>FI76</t>
+  </si>
+  <si>
+    <t>FI78</t>
+  </si>
+  <si>
+    <t>FI79</t>
+  </si>
+  <si>
+    <t>FI80</t>
+  </si>
+  <si>
+    <t>FI81</t>
+  </si>
+  <si>
+    <t>FI82</t>
+  </si>
+  <si>
+    <t>FI83</t>
+  </si>
+  <si>
+    <t>FI84</t>
+  </si>
+  <si>
+    <t>FI85</t>
+  </si>
+  <si>
+    <t>FI86</t>
+  </si>
+  <si>
+    <t>FI87</t>
+  </si>
+  <si>
+    <t>FI88</t>
+  </si>
+  <si>
+    <t>FI89</t>
+  </si>
+  <si>
+    <t>FI90</t>
+  </si>
+  <si>
+    <t>FI91</t>
+  </si>
+  <si>
+    <t>FI92</t>
+  </si>
+  <si>
+    <t>FI93</t>
+  </si>
+  <si>
+    <t>FI94</t>
+  </si>
+  <si>
+    <t>FI95</t>
   </si>
 </sst>
 </file>
@@ -230,9 +290,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -270,7 +330,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -376,7 +436,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -518,7 +578,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -870,10 +930,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860A3FB2-F49B-4E1A-98D6-8E64C29EF00A}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -902,7 +962,7 @@
       </c>
       <c r="B2">
         <f ca="1">0.4+RAND()/10</f>
-        <v>0.43688801914093245</v>
+        <v>0.47788014874167684</v>
       </c>
       <c r="C2">
         <v>1048.8987375520094</v>
@@ -917,7 +977,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B39" ca="1" si="0">0.4+RAND()/10</f>
-        <v>0.417795975145687</v>
+        <v>0.49575588821217303</v>
       </c>
       <c r="C3">
         <v>1015.9247665279173</v>
@@ -932,7 +992,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45904516284132113</v>
+        <v>0.40907834041670421</v>
       </c>
       <c r="C4">
         <v>1041.5899157282199</v>
@@ -947,7 +1007,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49386495126176522</v>
+        <v>0.42532509681164143</v>
       </c>
       <c r="C5">
         <v>1034.9351831687991</v>
@@ -962,7 +1022,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48222653270397087</v>
+        <v>0.46169565298112852</v>
       </c>
       <c r="C6">
         <v>1034.8201022056769</v>
@@ -977,7 +1037,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49044176269396944</v>
+        <v>0.4712971883371414</v>
       </c>
       <c r="C7">
         <v>1030.5111317389017</v>
@@ -992,7 +1052,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45378053293814441</v>
+        <v>0.40109561928535142</v>
       </c>
       <c r="C8">
         <v>1037.9505598725484</v>
@@ -1007,7 +1067,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49193174573715692</v>
+        <v>0.43741995061004169</v>
       </c>
       <c r="C9">
         <v>1015.7420222813428</v>
@@ -1022,7 +1082,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44491759971525835</v>
+        <v>0.44793464521210147</v>
       </c>
       <c r="C10">
         <v>1030.4199396576716</v>
@@ -1037,7 +1097,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49604250265848532</v>
+        <v>0.4015425860740206</v>
       </c>
       <c r="C11">
         <v>1006.8181662935915</v>
@@ -1052,7 +1112,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4999651493884455</v>
+        <v>0.49197232729469081</v>
       </c>
       <c r="C12">
         <v>1026.760566084811</v>
@@ -1067,7 +1127,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44783290899893585</v>
+        <v>0.41456008843101771</v>
       </c>
       <c r="C13">
         <v>1014.5437767254358</v>
@@ -1082,7 +1142,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43432032079970101</v>
+        <v>0.44058243066647179</v>
       </c>
       <c r="C14">
         <v>1014.5057860852271</v>
@@ -1097,7 +1157,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48987657806937557</v>
+        <v>0.41660396785754028</v>
       </c>
       <c r="C15">
         <v>1000.5222111680959</v>
@@ -1112,7 +1172,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44693263074506723</v>
+        <v>0.45265043684915335</v>
       </c>
       <c r="C16">
         <v>1044.7840400802461</v>
@@ -1127,7 +1187,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44759900013490939</v>
+        <v>0.4310184897995511</v>
       </c>
       <c r="C17">
         <v>1038.1072564377114</v>
@@ -1142,7 +1202,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46691232772085506</v>
+        <v>0.46731217671035441</v>
       </c>
       <c r="C18">
         <v>1003.0804891909572</v>
@@ -1157,7 +1217,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43681125381580832</v>
+        <v>0.4883468944285308</v>
       </c>
       <c r="C19">
         <v>1036.8645225471666</v>
@@ -1172,7 +1232,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4706250057516238</v>
+        <v>0.43569635275787044</v>
       </c>
       <c r="C20">
         <v>1007.3644263800718</v>
@@ -1187,7 +1247,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42626673678603577</v>
+        <v>0.46834020418406053</v>
       </c>
       <c r="C21">
         <v>1007.0276924038382</v>
@@ -1201,8 +1261,8 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.43724240909877954</v>
+        <f ca="1">0.2+RAND()/10</f>
+        <v>0.22225066433751139</v>
       </c>
       <c r="C22">
         <v>1034.068338439359</v>
@@ -1216,8 +1276,8 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.46653991580850246</v>
+        <f t="shared" ref="B23:B31" ca="1" si="1">0.2+RAND()/10</f>
+        <v>0.28805169519279389</v>
       </c>
       <c r="C23">
         <v>1025.5734052339465</v>
@@ -1231,8 +1291,8 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.48373019565959258</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.2501382146401791</v>
       </c>
       <c r="C24">
         <v>1040.442842954038</v>
@@ -1246,8 +1306,8 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.419152127235076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.23472568230519217</v>
       </c>
       <c r="C25">
         <v>1021.6881602500816</v>
@@ -1261,8 +1321,8 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.41426181419918678</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.27270444794800397</v>
       </c>
       <c r="C26">
         <v>1035.4802802553329</v>
@@ -1276,8 +1336,8 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.49377922887490933</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.20148326640079162</v>
       </c>
       <c r="C27">
         <v>1011.6447589751147</v>
@@ -1291,8 +1351,8 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.42512696704990982</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.22531132397695919</v>
       </c>
       <c r="C28">
         <v>1035.7310630756294</v>
@@ -1306,8 +1366,8 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.46012436931893236</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.27282107355440155</v>
       </c>
       <c r="C29">
         <v>1019.4447870413757</v>
@@ -1321,8 +1381,8 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.45442547835858743</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.29379968922202704</v>
       </c>
       <c r="C30">
         <v>1034.3244254204421</v>
@@ -1336,8 +1396,8 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.44083547839660486</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.21570002265483446</v>
       </c>
       <c r="C31">
         <v>1030.9788538090957</v>
@@ -1351,8 +1411,8 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.4130949155539872</v>
+        <f ca="1">0.8+RAND()/10</f>
+        <v>0.81552002550243974</v>
       </c>
       <c r="C32">
         <v>1019.6265168236124</v>
@@ -1366,8 +1426,8 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.43305833984673581</v>
+        <f t="shared" ref="B33:B38" ca="1" si="2">0.8+RAND()/10</f>
+        <v>0.89021824368024449</v>
       </c>
       <c r="C33">
         <v>1030.2698548116346</v>
@@ -1381,8 +1441,8 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.41417179991617487</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.85728201344108013</v>
       </c>
       <c r="C34">
         <v>1031.4276080201123</v>
@@ -1396,8 +1456,8 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.40041873149401319</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.87015179393359143</v>
       </c>
       <c r="C35">
         <v>1039.10639320633</v>
@@ -1411,8 +1471,8 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.40166102045343077</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.80538244942525306</v>
       </c>
       <c r="C36">
         <v>1030.959574308064</v>
@@ -1426,8 +1486,8 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.4270929298696502</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.87170979140915261</v>
       </c>
       <c r="C37">
         <v>1040.1105447404047</v>
@@ -1441,8 +1501,8 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.49007133475856501</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.84400971954852111</v>
       </c>
       <c r="C38">
         <v>1029.6585878004955</v>
@@ -1456,8 +1516,8 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.45812586127600197</v>
+        <f ca="1">0.1+RAND()/10</f>
+        <v>0.1511050197889148</v>
       </c>
       <c r="C39">
         <v>1000.948345450318</v>
@@ -1466,7 +1526,339 @@
         <v>0.80189669090063609</v>
       </c>
     </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40">
+        <f t="shared" ref="B40:B53" ca="1" si="3">0.1+RAND()/10</f>
+        <v>0.1029812005464974</v>
+      </c>
+      <c r="C40">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D40">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.11603745684769132</v>
+      </c>
+      <c r="C41">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D41">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.14200362817896134</v>
+      </c>
+      <c r="C42">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D42">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.14338299901137624</v>
+      </c>
+      <c r="C43">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D43">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.17675208513704438</v>
+      </c>
+      <c r="C44">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D44">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.19345887238251616</v>
+      </c>
+      <c r="C45">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D45">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.12411067331892228</v>
+      </c>
+      <c r="C46">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D46">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.15687493143559372</v>
+      </c>
+      <c r="C47">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D47">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.17306144883000643</v>
+      </c>
+      <c r="C48">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D48">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.14555700042358558</v>
+      </c>
+      <c r="C49">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D49">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.11012858454083291</v>
+      </c>
+      <c r="C50">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D50">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.18994348974775174</v>
+      </c>
+      <c r="C51">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D51">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52">
+        <f t="shared" ca="1" si="3"/>
+        <v>0.1664498769200094</v>
+      </c>
+      <c r="C52">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D52">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53">
+        <f ca="1">0.1+RAND()/10</f>
+        <v>0.19146882956900013</v>
+      </c>
+      <c r="C53">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D53">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54">
+        <f ca="1">0.05+RAND()/10</f>
+        <v>9.246668892451923E-2</v>
+      </c>
+      <c r="C54">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D54">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55">
+        <f t="shared" ref="B55:B61" ca="1" si="4">0.05+RAND()/10</f>
+        <v>7.3607677921353754E-2</v>
+      </c>
+      <c r="C55">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D55">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.10059073005629868</v>
+      </c>
+      <c r="C56">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D56">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57">
+        <f t="shared" ca="1" si="4"/>
+        <v>0.13939382240884451</v>
+      </c>
+      <c r="C57">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D57">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58">
+        <f t="shared" ca="1" si="4"/>
+        <v>6.4314820901032521E-2</v>
+      </c>
+      <c r="C58">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D58">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59">
+        <f t="shared" ca="1" si="4"/>
+        <v>6.9575582722719756E-2</v>
+      </c>
+      <c r="C59">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D59">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60">
+        <f t="shared" ca="1" si="4"/>
+        <v>8.0679493994688462E-2</v>
+      </c>
+      <c r="C60">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D60">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61">
+        <f>0.02</f>
+        <v>0.02</v>
+      </c>
+      <c r="C61">
+        <v>1000.948345450318</v>
+      </c>
+      <c r="D61">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final push for publicatoin v.1.0
</commit_message>
<xml_diff>
--- a/docs/Examples/EOS_calculations/Fluid_Inclusion_Densities_Example1.xlsx
+++ b/docs/Examples/EOS_calculations/Fluid_Inclusion_Densities_Example1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\Box\Berkeley_new\DiadFit_outer\docs\Examples\EOS_calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475E1E85-6E84-4A47-BE64-65311B263320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18BC7F3-28CF-4D7D-B15E-675362BF2964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3630" yWindow="90" windowWidth="20740" windowHeight="13400" activeTab="1" xr2:uid="{70B86B56-DC75-4A25-AC0B-5B934F645505}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{70B86B56-DC75-4A25-AC0B-5B934F645505}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
   <si>
     <t>Sample</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>FI95</t>
+  </si>
+  <si>
+    <t>XH2O</t>
   </si>
 </sst>
 </file>
@@ -930,19 +933,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860A3FB2-F49B-4E1A-98D6-8E64C29EF00A}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14.6328125" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="3" max="4" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -953,895 +956,1093 @@
         <v>42</v>
       </c>
       <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <f ca="1">0.4+RAND()/10</f>
-        <v>0.47788014874167684</v>
+        <v>0.45805451892516708</v>
       </c>
       <c r="C2">
         <v>1048.8987375520094</v>
       </c>
       <c r="D2">
+        <f ca="1">0.1-B2*0.03</f>
+        <v>8.6258364432244994E-2</v>
+      </c>
+      <c r="E2">
         <v>0.89779747510401875</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B39" ca="1" si="0">0.4+RAND()/10</f>
-        <v>0.49575588821217303</v>
+        <f t="shared" ref="B3:B21" ca="1" si="0">0.4+RAND()/10</f>
+        <v>0.49294749258651915</v>
       </c>
       <c r="C3">
         <v>1015.9247665279173</v>
       </c>
       <c r="D3">
+        <f t="shared" ref="D3:D19" ca="1" si="1">0.1-B3*0.03</f>
+        <v>8.5211575222404426E-2</v>
+      </c>
+      <c r="E3">
         <v>0.83184953305583464</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40907834041670421</v>
+        <v>0.48459440719443725</v>
       </c>
       <c r="C4">
         <v>1041.5899157282199</v>
       </c>
       <c r="D4">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.546216778416689E-2</v>
+      </c>
+      <c r="E4">
         <v>0.88317983145643986</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42532509681164143</v>
+        <v>0.49443112960195801</v>
       </c>
       <c r="C5">
         <v>1034.9351831687991</v>
       </c>
       <c r="D5">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.5167066111941261E-2</v>
+      </c>
+      <c r="E5">
         <v>0.86987036633759818</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46169565298112852</v>
+        <v>0.47641554936436742</v>
       </c>
       <c r="C6">
         <v>1034.8201022056769</v>
       </c>
       <c r="D6">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.5707533519068985E-2</v>
+      </c>
+      <c r="E6">
         <v>0.86964020441135381</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4712971883371414</v>
+        <v>0.44978504329745123</v>
       </c>
       <c r="C7">
         <v>1030.5111317389017</v>
       </c>
       <c r="D7">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.6506448701076474E-2</v>
+      </c>
+      <c r="E7">
         <v>0.86102226347780342</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40109561928535142</v>
+        <v>0.41480547420641539</v>
       </c>
       <c r="C8">
         <v>1037.9505598725484</v>
       </c>
       <c r="D8">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.7555835773807544E-2</v>
+      </c>
+      <c r="E8">
         <v>0.87590111974509688</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43741995061004169</v>
+        <v>0.45571975259962128</v>
       </c>
       <c r="C9">
         <v>1015.7420222813428</v>
       </c>
       <c r="D9">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.6328407422011366E-2</v>
+      </c>
+      <c r="E9">
         <v>0.83148404456268554</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44793464521210147</v>
+        <v>0.46068367207366534</v>
       </c>
       <c r="C10">
         <v>1030.4199396576716</v>
       </c>
       <c r="D10">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.6179489837790044E-2</v>
+      </c>
+      <c r="E10">
         <v>0.86083987931534334</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4015425860740206</v>
+        <v>0.44105588100710402</v>
       </c>
       <c r="C11">
         <v>1006.8181662935915</v>
       </c>
       <c r="D11">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.6768323569786893E-2</v>
+      </c>
+      <c r="E11">
         <v>0.81363633258718304</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49197232729469081</v>
+        <v>0.49575037716453862</v>
       </c>
       <c r="C12">
         <v>1026.760566084811</v>
       </c>
       <c r="D12">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.512748868506384E-2</v>
+      </c>
+      <c r="E12">
         <v>0.853521132169622</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41456008843101771</v>
+        <v>0.46460422426237175</v>
       </c>
       <c r="C13">
         <v>1014.5437767254358</v>
       </c>
       <c r="D13">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.6061873272128858E-2</v>
+      </c>
+      <c r="E13">
         <v>0.82908755345087171</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44058243066647179</v>
+        <v>0.41457750662653325</v>
       </c>
       <c r="C14">
         <v>1014.5057860852271</v>
       </c>
       <c r="D14">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.7562674801204013E-2</v>
+      </c>
+      <c r="E14">
         <v>0.82901157217045429</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41660396785754028</v>
+        <v>0.45331550925971664</v>
       </c>
       <c r="C15">
         <v>1000.5222111680959</v>
       </c>
       <c r="D15">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.6400534722208502E-2</v>
+      </c>
+      <c r="E15">
         <v>0.80104442233619177</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45265043684915335</v>
+        <v>0.46901444128508507</v>
       </c>
       <c r="C16">
         <v>1044.7840400802461</v>
       </c>
       <c r="D16">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.592956676144746E-2</v>
+      </c>
+      <c r="E16">
         <v>0.88956808016049216</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4310184897995511</v>
+        <v>0.42431354550816414</v>
       </c>
       <c r="C17">
         <v>1038.1072564377114</v>
       </c>
       <c r="D17">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.7270593634755089E-2</v>
+      </c>
+      <c r="E17">
         <v>0.87621451287542285</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46731217671035441</v>
+        <v>0.47653748523137796</v>
       </c>
       <c r="C18">
         <v>1003.0804891909572</v>
       </c>
       <c r="D18">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.5703875443058672E-2</v>
+      </c>
+      <c r="E18">
         <v>0.80616097838191447</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4883468944285308</v>
+        <v>0.48544429871218336</v>
       </c>
       <c r="C19">
         <v>1036.8645225471666</v>
       </c>
       <c r="D19">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.5436671038634504E-2</v>
+      </c>
+      <c r="E19">
         <v>0.87372904509433336</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43569635275787044</v>
+        <v>0.45488572003211686</v>
       </c>
       <c r="C20">
         <v>1007.3644263800718</v>
       </c>
       <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
         <v>0.81472885276014362</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46834020418406053</v>
+        <v>0.46934913230449171</v>
       </c>
       <c r="C21">
         <v>1007.0276924038382</v>
       </c>
       <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
         <v>0.81405538480767636</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22">
         <f ca="1">0.2+RAND()/10</f>
-        <v>0.22225066433751139</v>
+        <v>0.23256948206095701</v>
       </c>
       <c r="C22">
         <v>1034.068338439359</v>
       </c>
       <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
         <v>0.86813667687871798</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23">
-        <f t="shared" ref="B23:B31" ca="1" si="1">0.2+RAND()/10</f>
-        <v>0.28805169519279389</v>
+        <f t="shared" ref="B23:B31" ca="1" si="2">0.2+RAND()/10</f>
+        <v>0.20375885646539119</v>
       </c>
       <c r="C23">
         <v>1025.5734052339465</v>
       </c>
       <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
         <v>0.85114681046789298</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.2501382146401791</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.26623278578080373</v>
       </c>
       <c r="C24">
         <v>1040.442842954038</v>
       </c>
       <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
         <v>0.88088568590807614</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.23472568230519217</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.25205967595470652</v>
       </c>
       <c r="C25">
         <v>1021.6881602500816</v>
       </c>
       <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
         <v>0.84337632050016331</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.27270444794800397</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.20733031606911506</v>
       </c>
       <c r="C26">
         <v>1035.4802802553329</v>
       </c>
       <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
         <v>0.87096056051066584</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.20148326640079162</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.22782749665587987</v>
       </c>
       <c r="C27">
         <v>1011.6447589751147</v>
       </c>
       <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
         <v>0.82328951795022931</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.22531132397695919</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.2987138542931177</v>
       </c>
       <c r="C28">
         <v>1035.7310630756294</v>
       </c>
       <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
         <v>0.87146212615125895</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.27282107355440155</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.22487300536574673</v>
       </c>
       <c r="C29">
         <v>1019.4447870413757</v>
       </c>
       <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
         <v>0.83888957408275133</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.29379968922202704</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.2995018685216489</v>
       </c>
       <c r="C30">
         <v>1034.3244254204421</v>
       </c>
       <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
         <v>0.86864885084088428</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.21570002265483446</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.22831197028510597</v>
       </c>
       <c r="C31">
         <v>1030.9788538090957</v>
       </c>
       <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
         <v>0.86195770761819135</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32">
         <f ca="1">0.8+RAND()/10</f>
-        <v>0.81552002550243974</v>
+        <v>0.82393809930449735</v>
       </c>
       <c r="C32">
         <v>1019.6265168236124</v>
       </c>
       <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
         <v>0.83925303364722481</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33">
-        <f t="shared" ref="B33:B38" ca="1" si="2">0.8+RAND()/10</f>
-        <v>0.89021824368024449</v>
+        <f t="shared" ref="B33:B38" ca="1" si="3">0.8+RAND()/10</f>
+        <v>0.85256311900012083</v>
       </c>
       <c r="C33">
         <v>1030.2698548116346</v>
       </c>
       <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
         <v>0.8605397096232692</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.85728201344108013</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.85206577008536111</v>
       </c>
       <c r="C34">
         <v>1031.4276080201123</v>
       </c>
       <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
         <v>0.86285521604022464</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.87015179393359143</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.83034117357225146</v>
       </c>
       <c r="C35">
         <v>1039.10639320633</v>
       </c>
       <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
         <v>0.8782127864126601</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.80538244942525306</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.88285817105999265</v>
       </c>
       <c r="C36">
         <v>1030.959574308064</v>
       </c>
       <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
         <v>0.86191914861612806</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="B37">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.87170979140915261</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.89178378909637157</v>
       </c>
       <c r="C37">
         <v>1040.1105447404047</v>
       </c>
       <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
         <v>0.88022108948080957</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.84400971954852111</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.86071585847096765</v>
       </c>
       <c r="C38">
         <v>1029.6585878004955</v>
       </c>
       <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
         <v>0.85931717560099108</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
       <c r="B39">
         <f ca="1">0.1+RAND()/10</f>
-        <v>0.1511050197889148</v>
+        <v>0.14447106801978771</v>
       </c>
       <c r="C39">
         <v>1000.948345450318</v>
       </c>
       <c r="D39">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>44</v>
       </c>
       <c r="B40">
-        <f t="shared" ref="B40:B53" ca="1" si="3">0.1+RAND()/10</f>
-        <v>0.1029812005464974</v>
+        <f t="shared" ref="B40:B52" ca="1" si="4">0.1+RAND()/10</f>
+        <v>0.12741969130998784</v>
       </c>
       <c r="C40">
         <v>1000.948345450318</v>
       </c>
       <c r="D40">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.11603745684769132</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.12027425820689901</v>
       </c>
       <c r="C41">
         <v>1000.948345450318</v>
       </c>
       <c r="D41">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>45</v>
       </c>
       <c r="B42">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.14200362817896134</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.11804314309583161</v>
       </c>
       <c r="C42">
         <v>1000.948345450318</v>
       </c>
       <c r="D42">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>40</v>
       </c>
       <c r="B43">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.14338299901137624</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.10002109116748666</v>
       </c>
       <c r="C43">
         <v>1000.948345450318</v>
       </c>
       <c r="D43">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>46</v>
       </c>
       <c r="B44">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.17675208513704438</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.12552841925120389</v>
       </c>
       <c r="C44">
         <v>1000.948345450318</v>
       </c>
       <c r="D44">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>47</v>
       </c>
       <c r="B45">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.19345887238251616</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.14612538273646597</v>
       </c>
       <c r="C45">
         <v>1000.948345450318</v>
       </c>
       <c r="D45">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>48</v>
       </c>
       <c r="B46">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.12411067331892228</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.123014205756248</v>
       </c>
       <c r="C46">
         <v>1000.948345450318</v>
       </c>
       <c r="D46">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>49</v>
       </c>
       <c r="B47">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.15687493143559372</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.18042488187830039</v>
       </c>
       <c r="C47">
         <v>1000.948345450318</v>
       </c>
       <c r="D47">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>50</v>
       </c>
       <c r="B48">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.17306144883000643</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.18998294819391626</v>
       </c>
       <c r="C48">
         <v>1000.948345450318</v>
       </c>
       <c r="D48">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>51</v>
       </c>
       <c r="B49">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.14555700042358558</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.16889029565746605</v>
       </c>
       <c r="C49">
         <v>1000.948345450318</v>
       </c>
       <c r="D49">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>52</v>
       </c>
       <c r="B50">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.11012858454083291</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.14497170841501311</v>
       </c>
       <c r="C50">
         <v>1000.948345450318</v>
       </c>
       <c r="D50">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>53</v>
       </c>
       <c r="B51">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.18994348974775174</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.13397775086882169</v>
       </c>
       <c r="C51">
         <v>1000.948345450318</v>
       </c>
       <c r="D51">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>54</v>
       </c>
       <c r="B52">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.1664498769200094</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.12663118861576886</v>
       </c>
       <c r="C52">
         <v>1000.948345450318</v>
       </c>
       <c r="D52">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>55</v>
       </c>
       <c r="B53">
         <f ca="1">0.1+RAND()/10</f>
-        <v>0.19146882956900013</v>
+        <v>0.13948420629885122</v>
       </c>
       <c r="C53">
         <v>1000.948345450318</v>
       </c>
       <c r="D53">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>56</v>
       </c>
       <c r="B54">
         <f ca="1">0.05+RAND()/10</f>
-        <v>9.246668892451923E-2</v>
+        <v>0.12349449992009147</v>
       </c>
       <c r="C54">
         <v>1000.948345450318</v>
       </c>
       <c r="D54">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>57</v>
       </c>
       <c r="B55">
-        <f t="shared" ref="B55:B61" ca="1" si="4">0.05+RAND()/10</f>
-        <v>7.3607677921353754E-2</v>
+        <f t="shared" ref="B55:B60" ca="1" si="5">0.05+RAND()/10</f>
+        <v>0.12782411615396261</v>
       </c>
       <c r="C55">
         <v>1000.948345450318</v>
       </c>
       <c r="D55">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>58</v>
       </c>
       <c r="B56">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.10059073005629868</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.10952152200655443</v>
       </c>
       <c r="C56">
         <v>1000.948345450318</v>
       </c>
       <c r="D56">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>59</v>
       </c>
       <c r="B57">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.13939382240884451</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>6.4134662074698742E-2</v>
       </c>
       <c r="C57">
         <v>1000.948345450318</v>
       </c>
       <c r="D57">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>60</v>
       </c>
       <c r="B58">
-        <f t="shared" ca="1" si="4"/>
-        <v>6.4314820901032521E-2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>5.5106054412405341E-2</v>
       </c>
       <c r="C58">
         <v>1000.948345450318</v>
       </c>
       <c r="D58">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>61</v>
       </c>
       <c r="B59">
-        <f t="shared" ca="1" si="4"/>
-        <v>6.9575582722719756E-2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>7.0195134342481216E-2</v>
       </c>
       <c r="C59">
         <v>1000.948345450318</v>
       </c>
       <c r="D59">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>62</v>
       </c>
       <c r="B60">
-        <f t="shared" ca="1" si="4"/>
-        <v>8.0679493994688462E-2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.12098266211360088</v>
       </c>
       <c r="C60">
         <v>1000.948345450318</v>
       </c>
       <c r="D60">
-        <v>0.80189669090063609</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0.80189669090063609</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -1853,6 +2054,9 @@
         <v>1000.948345450318</v>
       </c>
       <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
         <v>0.80189669090063609</v>
       </c>
     </row>

</xml_diff>